<commit_message>
use 5 digit format with leading zero
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhoga\Desktop\yhogakafi.github.io\import pesanan penjualan\xlsx_to_xml_converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AC87B5-DA07-424A-99A9-5DDFCB61DE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C9A784-889D-4114-9BDE-68B71B35F9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F016DAE-7158-43ED-93F7-D86C285BF227}"/>
   </bookViews>
@@ -258,7 +258,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,16 +424,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -457,7 +457,37 @@
     <cellStyle name="S8" xfId="9" xr:uid="{5BF649B2-4165-4105-BBC2-EF84D15053CA}"/>
     <cellStyle name="S9" xfId="10" xr:uid="{38525B38-F572-46ED-8262-49647F32C67D}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -801,64 +831,64 @@
   <dimension ref="A1:BJ2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="21" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="21" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16" customWidth="1"/>
-    <col min="25" max="25" width="11.28515625" customWidth="1"/>
-    <col min="26" max="26" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.25" customWidth="1"/>
+    <col min="26" max="26" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.75" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.42578125" customWidth="1"/>
-    <col min="33" max="34" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.375" customWidth="1"/>
+    <col min="33" max="34" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="8" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="29.375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="33.375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="34.375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="33.625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="3.625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9.75" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="18" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" ht="60">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1076,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:62" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" s="5" customFormat="1" ht="30">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1133,7 +1163,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="W1:W1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="grosir">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="grosir">
       <formula>NOT(ISERROR(SEARCH("grosir",W1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1150,7 +1180,7 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>